<commit_message>
4 scripts in xml
</commit_message>
<xml_diff>
--- a/testData/SFS_AllMobile_Tbl_RThree.xlsx
+++ b/testData/SFS_AllMobile_Tbl_RThree.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="144">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -427,6 +427,30 @@
   </si>
   <si>
     <t>formshow_16112023</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:10 AM to 09:14 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:15 AM to 09:19 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:20 AM to 09:24 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:25 AM to 09:29 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:30 AM to 09:34 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:35 AM to 09:39 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:40 AM to 09:44 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:45 AM to 09:49 AM ]</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1040,7 @@
         <v>50</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="P2" t="s" s="0">
         <v>51</v>

</xml_diff>